<commit_message>
2022.7.14 21.37 for textures
</commit_message>
<xml_diff>
--- a/sunken_world_project.xlsx
+++ b/sunken_world_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbydd\Documents\gitProject\SunkenWorld\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hqyzsy\IdeaProjects\Sunken-World\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39211E86-1AA6-46E2-81E3-D44439E53D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C05E20-6DB5-48EE-8B31-82850DD4EBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{9F1E8E19-7F12-4D94-A84A-B6D4AB5447D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{9F1E8E19-7F12-4D94-A84A-B6D4AB5447D3}"/>
   </bookViews>
   <sheets>
     <sheet name="注释" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
   <si>
     <t>循环呼吸器</t>
   </si>
@@ -404,17 +404,45 @@
   </si>
   <si>
     <t>碰撞箱高宽0.5</t>
+  </si>
+  <si>
+    <t>红珊瑚</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>四周需要有完整方块依附，否则会脱落</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>有四个方向</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>red_coral</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>海蘑菇</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sea_shroom</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>下方方块为砂砾</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -422,15 +450,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -824,40 +859,41 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B6" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -871,14 +907,14 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -886,7 +922,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -894,7 +930,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -902,7 +938,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -910,7 +946,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
@@ -918,7 +954,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -926,7 +962,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>94</v>
       </c>
@@ -934,7 +970,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>95</v>
       </c>
@@ -942,7 +978,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>98</v>
       </c>
@@ -951,28 +987,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9745FCB9-6E30-4484-A5FA-5F21001E229E}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
@@ -987,7 +1024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1001,7 +1038,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1010,7 +1047,7 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>108</v>
       </c>
@@ -1023,12 +1060,12 @@
       </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -1040,7 +1077,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1051,7 +1088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1063,13 +1100,40 @@
       </c>
       <c r="D9" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E2:E3"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1081,9 +1145,9 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>110</v>
       </c>
@@ -1094,12 +1158,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1112,13 +1177,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -1126,7 +1191,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
@@ -1134,13 +1199,14 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1149,13 +1215,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D915CF-F878-49C2-B7D6-286849B6BDEF}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
@@ -1163,7 +1229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +1237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1187,7 +1253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>118</v>
       </c>
@@ -1207,6 +1273,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1216,19 +1283,19 @@
   <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="90.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -1242,7 +1309,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1323,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1273,7 +1340,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1292,7 +1359,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1311,7 +1378,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1392,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1406,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1353,7 +1420,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>91</v>
       </c>
@@ -1368,7 +1435,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1383,7 +1450,7 @@
       </c>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>92</v>
       </c>
@@ -1398,7 +1465,7 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>100</v>
       </c>
@@ -1413,7 +1480,7 @@
       </c>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>104</v>
       </c>
@@ -1435,6 +1502,7 @@
   <mergeCells count="1">
     <mergeCell ref="G11:G13"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1447,21 +1515,21 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1478,7 +1546,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1487,6 +1555,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{67794910-14B1-437B-AA1E-3E7E6BE04F93}"/>
   </hyperlinks>
@@ -1502,14 +1571,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -1520,17 +1589,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
@@ -1538,27 +1607,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>